<commit_message>
Import topic csv file, however wordcloud needs to be built
</commit_message>
<xml_diff>
--- a/src/data/dashboard_data.xlsx
+++ b/src/data/dashboard_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Personal)\My projects\CRRC\SIDA dashboard\dashboard\sm_monitoring\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350D5580-7F6D-4164-A9D8-00C84F56196F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D232CD-353D-4C84-BE6D-6195BA22F71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="ნარატივები" sheetId="2" r:id="rId2"/>
     <sheet name="აქტორები" sheetId="3" r:id="rId3"/>
     <sheet name="თემა" sheetId="4" r:id="rId4"/>
+    <sheet name="მოვლენები" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$W$116</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="885">
   <si>
     <t>#</t>
   </si>
@@ -2480,6 +2481,237 @@
   </si>
   <si>
     <t>actor_text</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>გიორგობა</t>
+  </si>
+  <si>
+    <t>ბარბარობა</t>
+  </si>
+  <si>
+    <t>ახალი წელი</t>
+  </si>
+  <si>
+    <t>შობა</t>
+  </si>
+  <si>
+    <t>Keyword. საკვანძო სიტყვები ტექსტიდან, რაც ანტი-დასავლურ ნარატივს მიესადაგება (ფორმატი: მხოლოდ მძიმე. მაგალითად: უსამშობლო,ტვინგარეცხილი,მოღალატე სტუდენტობა)</t>
+  </si>
+  <si>
+    <t>ძარცვა</t>
+  </si>
+  <si>
+    <t>ველური ნაცები</t>
+  </si>
+  <si>
+    <t>აგრესიული დაჯგუფება, რადიკალური დაჯგუფება</t>
+  </si>
+  <si>
+    <t>რადიკალური დაჯგუფება</t>
+  </si>
+  <si>
+    <t>რადიკალების აქცია</t>
+  </si>
+  <si>
+    <t>რადიკალური ჯგუფების კოორდინირება</t>
+  </si>
+  <si>
+    <t>მტრების პროპაგანდა,სამოქალაქო ომი,ძმათა სისხლისღვრა</t>
+  </si>
+  <si>
+    <t>აგრესიული რადიკალები,დაქირავებული რუსები და უკრაინელები</t>
+  </si>
+  <si>
+    <t>რუსკი ხოშტარია,ოკუპანტის ენა</t>
+  </si>
+  <si>
+    <t>წარსულში ქურდობისთვის ნასამართლევი,ცეცხლის წაკიდებით ნივთის დაზიანება,ნარკოტიკული საშუალების უკანონო შეძენა-შენახვისთვის ნასამართლევი</t>
+  </si>
+  <si>
+    <t>შიდა მტრები,ძმათა სისხლისღვრა,უცხო ქვეყნის დავალება,უცხო ქვეყნის დაფინანსება</t>
+  </si>
+  <si>
+    <t>ძმათა სისხლისღვრა,ქვეყნის მტრები</t>
+  </si>
+  <si>
+    <t>დააზიანე შენი სამშობლო</t>
+  </si>
+  <si>
+    <t>რადიკალური ექსტრემისტები</t>
+  </si>
+  <si>
+    <t>ამდენი ბავშვი, არასრულწლოვნები</t>
+  </si>
+  <si>
+    <t>ოპოზიციის არამშვიდობიანი აქცია,დაშავებული პოლიციელი</t>
+  </si>
+  <si>
+    <t>ევროკავშირის შანტაჟი,ხელოვნური ინსტრუმენტი,საზოგადოების პოლარიზაცია,რადიკალიზმის გაღვივება</t>
+  </si>
+  <si>
+    <t>თავდასხმა პოლიციელებზე,მერიის ქონების დაზიანება</t>
+  </si>
+  <si>
+    <t>ბარიკადები</t>
+  </si>
+  <si>
+    <t>სასტიკი ძალადობა,დასავლელი სპონსორები,რადიკალური ოპოზიცია,მოძალადეების შეკრება</t>
+  </si>
+  <si>
+    <t>აგენტურა, მეხუთე კოლონა</t>
+  </si>
+  <si>
+    <t>კონფრონტაცია,შეურაცხყოფა</t>
+  </si>
+  <si>
+    <t>დაამტვრიეს,ქვები ისროლეს</t>
+  </si>
+  <si>
+    <t>ძალადობრივი ქმედებები,"მშვიდობიანი"</t>
+  </si>
+  <si>
+    <t>უცხოელი ინსტრუქტორები</t>
+  </si>
+  <si>
+    <t>მოლოტობის კოქტეილი</t>
+  </si>
+  <si>
+    <t>"მშვიდობიანი"</t>
+  </si>
+  <si>
+    <t>ცეცხლი წაუკიდეს</t>
+  </si>
+  <si>
+    <t>უხეში შანტაჟი</t>
+  </si>
+  <si>
+    <t>ძალადობრივი ქმედებები</t>
+  </si>
+  <si>
+    <t>გვამი გვჭირდება,"მკვლელი სახელმწიფო"</t>
+  </si>
+  <si>
+    <t>გარე დაფინანსება</t>
+  </si>
+  <si>
+    <t>გვამი გვჭირდება,</t>
+  </si>
+  <si>
+    <t>არეულობის მონაწილე</t>
+  </si>
+  <si>
+    <t>სისხლისმსმელი, მაიდანი, მეორე ფრონტი</t>
+  </si>
+  <si>
+    <t>ურჯულოები</t>
+  </si>
+  <si>
+    <t>სამშობლოს მტრები</t>
+  </si>
+  <si>
+    <t>რევოლუციას მოწყურებული ჯენზი, მოღალატე, არაკაცი, სისხლი სწყურია ბიჭს</t>
+  </si>
+  <si>
+    <t>მოღალატე</t>
+  </si>
+  <si>
+    <t>შანტაჟი</t>
+  </si>
+  <si>
+    <t>სამშობლოზე სროლა</t>
+  </si>
+  <si>
+    <t>ბლადიმირ დოუნდობელი</t>
+  </si>
+  <si>
+    <t>სატანის თაყვანისმცემლები, სულს ყიდიან</t>
+  </si>
+  <si>
+    <t>"პროდასავლელი" ტერორისტები, რევოლუციურ-საბოტაჟური მასკარადი</t>
+  </si>
+  <si>
+    <t>განსხვავებული აზრის დევნა, ეკლესიას აგინებენ, პატრიარქს აგინებენ, უნამუსოები, ქვეყნის გამყიდველები</t>
+  </si>
+  <si>
+    <t>მანქურთები</t>
+  </si>
+  <si>
+    <t>გრინჩები</t>
+  </si>
+  <si>
+    <t>დასავლეთის მონები, აგრესიული მომიტინგეები</t>
+  </si>
+  <si>
+    <t>პატიმრების წამება,მკვლელობა, ცემა, ექსტრადირება</t>
+  </si>
+  <si>
+    <t>ცენზურა</t>
+  </si>
+  <si>
+    <t>ნაცმაიდანი,მოვერევით,არ დავუშვებთ,არ დავუშვათ,ნაცები,</t>
+  </si>
+  <si>
+    <t>გახსენით-ვაწერთ!,შანტაჟის გარეშე,ღირსებით</t>
+  </si>
+  <si>
+    <t>არერულობა, რევოლუცია, ბულინგი,</t>
+  </si>
+  <si>
+    <t>საქართველოს ანჯღრევენ,მიზანმიმართულად ანჯღრევენ,შიდა და გარე მტრები,პირადი ინტერესები,უსამშობლო ადამიანები,ქვეყნის მტრობა,დაქუცმაცება,ქვეყანა იშლება,ნადგურდება,საშინელების ორგანიზატორები,დამღუპველი მარშები,</t>
+  </si>
+  <si>
+    <t>გვებრძვიან,ქართულ სიტყვას ახშობენ,</t>
+  </si>
+  <si>
+    <t>ქართული ოცნების დამსახურებაა,ნაცების ორგანიზებული აქცია,არ არსებობდა თავისუფალი მედია,თქვენ თანატოლებს აუპატიურებდნენ,ორი ვარიანტი,მათ ორგანიზებულ აქციაზე დგახარ,შვილო,ვერ დავუშვებთ მათ მობრუნმებას,წარმოდგენა არ გაქვს,თავისუფლებას არავინ გართმევთ,ცუდად გიყენებ,გატყუებენ</t>
+  </si>
+  <si>
+    <t>არ დავუშვებთ,</t>
+  </si>
+  <si>
+    <t>ამათი გადატრიალებული, არ გაიშვას,ამათ აქციაზე,როგორ დადიხართ,</t>
+  </si>
+  <si>
+    <t>გასამართლება,ნაციონალური მოძრაობა</t>
+  </si>
+  <si>
+    <t>ნაცებო,მიიღო საკადრისი,დარეკა პოლიციაში,ფურცელი ვერ გააგდებინეს</t>
+  </si>
+  <si>
+    <t>ვთრთით თქვენი შიშით</t>
+  </si>
+  <si>
+    <t>მიშადან მზიამდე,</t>
+  </si>
+  <si>
+    <t>მუქარა</t>
+  </si>
+  <si>
+    <t>პიროტექნიკა,ხლაპუშკები</t>
+  </si>
+  <si>
+    <t>კრემლის მყისიერი შექება,დასავლეთის ინტეგრაციის გზიდან გადახვევა</t>
+  </si>
+  <si>
+    <t>მეხუთე კოლონა,ევროპის შესაბამისი ბიუროკრატები,რადიკალები და მათი უცხოელი მფარველები, უკრაინად გადაქცევა</t>
+  </si>
+  <si>
+    <t>საქართველოს უკრაინიზაცია,საზოგადოების გახლეჩა</t>
+  </si>
+  <si>
+    <t>დივერსიული ჯგუფები,ომია</t>
+  </si>
+  <si>
+    <t>აგრესიული მომიტინგები</t>
+  </si>
+  <si>
+    <t>ურტყავთ!?</t>
   </si>
 </sst>
 </file>
@@ -3080,14 +3312,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="5" max="11" width="11.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3157,8 +3389,11 @@
       <c r="W1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X1" s="4" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3208,8 +3443,9 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="8"/>
-    </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3251,8 +3487,9 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="8"/>
-    </row>
-    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3296,8 +3533,11 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="8"/>
-    </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X4" s="8" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3351,8 +3591,11 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="8"/>
-    </row>
-    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X5" s="8" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3402,8 +3645,11 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="8"/>
-    </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X6" s="8" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3453,8 +3699,11 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="8"/>
-    </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X7" s="8" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3504,8 +3753,9 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="8"/>
-    </row>
-    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3555,8 +3805,9 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="8"/>
-    </row>
-    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3612,8 +3863,11 @@
       <c r="W10" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X10" s="8" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3665,8 +3919,11 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="8"/>
-    </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X11" s="8" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3722,8 +3979,11 @@
       <c r="W12" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X12" s="8" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3783,8 +4043,11 @@
       <c r="W13" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X13" s="8" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3834,8 +4097,11 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="8"/>
-    </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X14" s="8" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3895,8 +4161,11 @@
       <c r="W15" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X15" s="8" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3944,8 +4213,11 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="8"/>
-    </row>
-    <row r="17" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X16" s="8" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3995,8 +4267,11 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="8"/>
-    </row>
-    <row r="18" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X17" s="8" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -4040,8 +4315,11 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="8"/>
-    </row>
-    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X18" s="8" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -4089,8 +4367,11 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="8"/>
-    </row>
-    <row r="20" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X19" s="8" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -4142,8 +4423,9 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="8"/>
-    </row>
-    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -4193,8 +4475,9 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="8"/>
-    </row>
-    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -4238,8 +4521,9 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="8"/>
-    </row>
-    <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -4299,8 +4583,11 @@
       <c r="W23" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X23" s="8" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -4356,8 +4643,11 @@
       <c r="W24" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X24" s="13" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -4407,8 +4697,11 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="8"/>
-    </row>
-    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X25" s="8" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -4466,8 +4759,11 @@
       <c r="W26" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X26" s="8" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -4517,8 +4813,11 @@
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="8"/>
-    </row>
-    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X27" s="8" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -4580,8 +4879,11 @@
       <c r="W28" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X28" s="8" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -4637,8 +4939,11 @@
       <c r="W29" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X29" s="8" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -4688,8 +4993,11 @@
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="8"/>
-    </row>
-    <row r="31" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X30" s="8" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -4739,8 +5047,9 @@
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
       <c r="W31" s="8"/>
-    </row>
-    <row r="32" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -4790,8 +5099,11 @@
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="8"/>
-    </row>
-    <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X32" s="8" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -4835,8 +5147,11 @@
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
       <c r="W33" s="8"/>
-    </row>
-    <row r="34" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X33" s="8" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -4888,8 +5203,11 @@
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
       <c r="W34" s="8"/>
-    </row>
-    <row r="35" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X34" s="8" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -4939,8 +5257,11 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="8"/>
-    </row>
-    <row r="36" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X35" s="8" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -4984,8 +5305,11 @@
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="8"/>
-    </row>
-    <row r="37" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X36" s="8" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -5029,8 +5353,9 @@
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
       <c r="W37" s="8"/>
-    </row>
-    <row r="38" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X37" s="8"/>
+    </row>
+    <row r="38" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -5074,8 +5399,9 @@
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
       <c r="W38" s="8"/>
-    </row>
-    <row r="39" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -5125,8 +5451,11 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
       <c r="W39" s="8"/>
-    </row>
-    <row r="40" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X39" s="8" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -5170,8 +5499,11 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="8"/>
-    </row>
-    <row r="41" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X40" s="8" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -5231,8 +5563,11 @@
       <c r="W41" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X41" s="8" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -5282,8 +5617,11 @@
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
       <c r="W42" s="8"/>
-    </row>
-    <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X42" s="8" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -5339,8 +5677,11 @@
       <c r="W43" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X43" s="8" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -5390,8 +5731,11 @@
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="8"/>
-    </row>
-    <row r="45" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X44" s="8" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -5447,8 +5791,11 @@
       <c r="W45" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X45" s="8" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -5498,8 +5845,11 @@
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
       <c r="W46" s="8"/>
-    </row>
-    <row r="47" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X46" s="8" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -5555,8 +5905,9 @@
       <c r="W47" s="13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X47" s="13"/>
+    </row>
+    <row r="48" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -5606,8 +5957,11 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="8"/>
-    </row>
-    <row r="49" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X48" s="8" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -5659,8 +6013,11 @@
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
       <c r="W49" s="8"/>
-    </row>
-    <row r="50" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X49" s="8" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -5706,8 +6063,9 @@
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
       <c r="W50" s="8"/>
-    </row>
-    <row r="51" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X50" s="8"/>
+    </row>
+    <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -5753,8 +6111,9 @@
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
       <c r="W51" s="8"/>
-    </row>
-    <row r="52" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X51" s="8"/>
+    </row>
+    <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -5802,8 +6161,11 @@
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
       <c r="W52" s="8"/>
-    </row>
-    <row r="53" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X52" s="8" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -5857,8 +6219,11 @@
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
       <c r="W53" s="8"/>
-    </row>
-    <row r="54" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X53" s="8" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -5908,8 +6273,11 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
       <c r="W54" s="8"/>
-    </row>
-    <row r="55" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X54" s="8" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -5963,8 +6331,9 @@
       <c r="U55" s="6"/>
       <c r="V55" s="6"/>
       <c r="W55" s="8"/>
-    </row>
-    <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X55" s="8"/>
+    </row>
+    <row r="56" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -6016,8 +6385,11 @@
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
       <c r="W56" s="8"/>
-    </row>
-    <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X56" s="8" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -6073,8 +6445,9 @@
       <c r="W57" s="8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="58" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X57" s="8"/>
+    </row>
+    <row r="58" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -6132,8 +6505,9 @@
       <c r="W58" s="8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="59" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X58" s="8"/>
+    </row>
+    <row r="59" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -6197,8 +6571,11 @@
       <c r="W59" s="8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X59" s="8" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -6260,8 +6637,11 @@
       <c r="W60" s="8" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="61" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X60" s="8" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -6313,8 +6693,11 @@
       <c r="U61" s="6"/>
       <c r="V61" s="6"/>
       <c r="W61" s="8"/>
-    </row>
-    <row r="62" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X61" s="8" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6366,8 +6749,9 @@
       <c r="U62" s="6"/>
       <c r="V62" s="6"/>
       <c r="W62" s="8"/>
-    </row>
-    <row r="63" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X62" s="8"/>
+    </row>
+    <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -6427,8 +6811,11 @@
       <c r="W63" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="64" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X63" s="8" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -6494,8 +6881,11 @@
       <c r="W64" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="65" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X64" s="8" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -6539,8 +6929,11 @@
       <c r="U65" s="6"/>
       <c r="V65" s="6"/>
       <c r="W65" s="8"/>
-    </row>
-    <row r="66" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X65" s="8" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -6608,8 +7001,11 @@
       <c r="W66" s="8" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X66" s="8" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -6671,8 +7067,11 @@
       <c r="W67" s="8" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="68" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X67" s="8" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -6728,8 +7127,11 @@
       <c r="U68" s="6"/>
       <c r="V68" s="6"/>
       <c r="W68" s="8"/>
-    </row>
-    <row r="69" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X68" s="8" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6793,8 +7195,11 @@
       <c r="W69" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="70" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X69" s="8" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -6858,8 +7263,11 @@
       <c r="W70" s="20" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="71" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X70" s="20" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6909,8 +7317,11 @@
       <c r="U71" s="24"/>
       <c r="V71" s="24"/>
       <c r="W71" s="24"/>
-    </row>
-    <row r="72" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X71" s="24" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -6964,8 +7375,11 @@
       <c r="U72" s="24"/>
       <c r="V72" s="24"/>
       <c r="W72" s="24"/>
-    </row>
-    <row r="73" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X72" s="24" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -7031,8 +7445,11 @@
       <c r="W73" s="24" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="74" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X73" s="24" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -7066,8 +7483,9 @@
       <c r="U74" s="24"/>
       <c r="V74" s="24"/>
       <c r="W74" s="24"/>
-    </row>
-    <row r="75" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X74" s="24"/>
+    </row>
+    <row r="75" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -7111,8 +7529,11 @@
       <c r="U75" s="24"/>
       <c r="V75" s="24"/>
       <c r="W75" s="24"/>
-    </row>
-    <row r="76" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X75" s="24" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -7176,8 +7597,11 @@
       <c r="W76" s="24" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="77" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X76" s="24" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -7223,8 +7647,9 @@
       <c r="U77" s="24"/>
       <c r="V77" s="24"/>
       <c r="W77" s="24"/>
-    </row>
-    <row r="78" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X77" s="24"/>
+    </row>
+    <row r="78" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -7272,8 +7697,11 @@
       <c r="U78" s="24"/>
       <c r="V78" s="24"/>
       <c r="W78" s="24"/>
-    </row>
-    <row r="79" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X78" s="24" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -7307,8 +7735,9 @@
       <c r="U79" s="24"/>
       <c r="V79" s="24"/>
       <c r="W79" s="24"/>
-    </row>
-    <row r="80" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X79" s="24"/>
+    </row>
+    <row r="80" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -7342,6 +7771,7 @@
       <c r="U80" s="24"/>
       <c r="V80" s="24"/>
       <c r="W80" s="24"/>
+      <c r="X80" s="24"/>
     </row>
     <row r="81" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A81" s="5">
@@ -7395,6 +7825,9 @@
       <c r="U81" s="24"/>
       <c r="V81" s="24"/>
       <c r="W81" s="24"/>
+      <c r="X81" s="24" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="82" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A82" s="5">
@@ -7440,6 +7873,7 @@
       <c r="U82" s="24"/>
       <c r="V82" s="24"/>
       <c r="W82" s="24"/>
+      <c r="X82" s="24"/>
     </row>
     <row r="83" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
@@ -7485,6 +7919,7 @@
       <c r="U83" s="24"/>
       <c r="V83" s="24"/>
       <c r="W83" s="24"/>
+      <c r="X83" s="24"/>
     </row>
     <row r="84" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A84" s="5">
@@ -7538,6 +7973,7 @@
       <c r="U84" s="24"/>
       <c r="V84" s="24"/>
       <c r="W84" s="24"/>
+      <c r="X84" s="24"/>
     </row>
     <row r="85" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
@@ -7583,6 +8019,9 @@
       <c r="U85" s="24"/>
       <c r="V85" s="24"/>
       <c r="W85" s="24"/>
+      <c r="X85" s="24" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="86" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A86" s="5">
@@ -7630,6 +8069,7 @@
       <c r="U86" s="24"/>
       <c r="V86" s="24"/>
       <c r="W86" s="24"/>
+      <c r="X86" s="24"/>
     </row>
     <row r="87" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
@@ -7693,6 +8133,7 @@
       <c r="W87" s="24" t="s">
         <v>191</v>
       </c>
+      <c r="X87" s="24"/>
     </row>
     <row r="88" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A88" s="5">
@@ -7738,6 +8179,7 @@
       <c r="U88" s="24"/>
       <c r="V88" s="24"/>
       <c r="W88" s="24"/>
+      <c r="X88" s="24"/>
     </row>
     <row r="89" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
@@ -7802,6 +8244,9 @@
       </c>
       <c r="W89" s="24" t="s">
         <v>195</v>
+      </c>
+      <c r="X89" s="24" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="90" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -7838,6 +8283,7 @@
       <c r="U90" s="24"/>
       <c r="V90" s="24"/>
       <c r="W90" s="24"/>
+      <c r="X90" s="24"/>
     </row>
     <row r="91" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
@@ -7885,6 +8331,9 @@
       <c r="U91" s="24"/>
       <c r="V91" s="24"/>
       <c r="W91" s="24"/>
+      <c r="X91" s="24" t="s">
+        <v>875</v>
+      </c>
     </row>
     <row r="92" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A92" s="5">
@@ -7940,6 +8389,9 @@
       <c r="U92" s="24"/>
       <c r="V92" s="24"/>
       <c r="W92" s="24"/>
+      <c r="X92" s="24" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="93" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A93" s="5">
@@ -7975,6 +8427,7 @@
       <c r="U93" s="24"/>
       <c r="V93" s="24"/>
       <c r="W93" s="24"/>
+      <c r="X93" s="24"/>
     </row>
     <row r="94" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A94" s="5">
@@ -8036,7 +8489,9 @@
       <c r="W94" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="X94" s="6"/>
+      <c r="X94" s="13" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="95" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A95" s="5">
@@ -8084,7 +8539,7 @@
       <c r="U95" s="6"/>
       <c r="V95" s="6"/>
       <c r="W95" s="8"/>
-      <c r="X95" s="6"/>
+      <c r="X95" s="8"/>
     </row>
     <row r="96" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A96" s="5">
@@ -8130,7 +8585,9 @@
       <c r="U96" s="6"/>
       <c r="V96" s="6"/>
       <c r="W96" s="8"/>
-      <c r="X96" s="6"/>
+      <c r="X96" s="8" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="97" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="5">
@@ -8244,7 +8701,7 @@
       <c r="W98" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="X98" s="6"/>
+      <c r="X98" s="8"/>
     </row>
     <row r="99" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
@@ -8298,7 +8755,7 @@
       <c r="U99" s="6"/>
       <c r="V99" s="6"/>
       <c r="W99" s="8"/>
-      <c r="X99" s="6"/>
+      <c r="X99" s="8"/>
     </row>
     <row r="100" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A100" s="5">
@@ -8344,7 +8801,7 @@
       <c r="U100" s="6"/>
       <c r="V100" s="6"/>
       <c r="W100" s="8"/>
-      <c r="X100" s="6"/>
+      <c r="X100" s="8"/>
     </row>
     <row r="101" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
@@ -8398,7 +8855,7 @@
       <c r="U101" s="6"/>
       <c r="V101" s="6"/>
       <c r="W101" s="8"/>
-      <c r="X101" s="6"/>
+      <c r="X101" s="8"/>
     </row>
     <row r="102" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A102" s="5">
@@ -8444,7 +8901,7 @@
       <c r="U102" s="6"/>
       <c r="V102" s="6"/>
       <c r="W102" s="8"/>
-      <c r="X102" s="6"/>
+      <c r="X102" s="8"/>
     </row>
     <row r="103" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
@@ -8504,7 +8961,7 @@
       <c r="W103" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="X103" s="6"/>
+      <c r="X103" s="8"/>
     </row>
     <row r="104" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A104" s="5">
@@ -8556,7 +9013,9 @@
       <c r="U104" s="6"/>
       <c r="V104" s="6"/>
       <c r="W104" s="8"/>
-      <c r="X104" s="6"/>
+      <c r="X104" s="8" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="105" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
@@ -8608,7 +9067,7 @@
       <c r="U105" s="6"/>
       <c r="V105" s="6"/>
       <c r="W105" s="8"/>
-      <c r="X105" s="6"/>
+      <c r="X105" s="8"/>
     </row>
     <row r="106" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A106" s="5">
@@ -8670,7 +9129,7 @@
       <c r="W106" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="X106" s="6"/>
+      <c r="X106" s="8"/>
     </row>
     <row r="107" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
@@ -8722,7 +9181,9 @@
       <c r="U107" s="6"/>
       <c r="V107" s="6"/>
       <c r="W107" s="8"/>
-      <c r="X107" s="6"/>
+      <c r="X107" s="8" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="108" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="5">
@@ -8784,7 +9245,9 @@
       <c r="W108" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="X108" s="6"/>
+      <c r="X108" s="8" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="109" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
@@ -8836,7 +9299,7 @@
       <c r="U109" s="6"/>
       <c r="V109" s="6"/>
       <c r="W109" s="8"/>
-      <c r="X109" s="6"/>
+      <c r="X109" s="8"/>
     </row>
     <row r="110" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="5">
@@ -8888,7 +9351,9 @@
       <c r="U110" s="6"/>
       <c r="V110" s="6"/>
       <c r="W110" s="8"/>
-      <c r="X110" s="6"/>
+      <c r="X110" s="8" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="111" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A111" s="5">
@@ -8934,7 +9399,7 @@
       <c r="U111" s="6"/>
       <c r="V111" s="6"/>
       <c r="W111" s="8"/>
-      <c r="X111" s="6"/>
+      <c r="X111" s="8"/>
     </row>
     <row r="112" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A112" s="5">
@@ -8980,7 +9445,7 @@
       <c r="U112" s="6"/>
       <c r="V112" s="6"/>
       <c r="W112" s="8"/>
-      <c r="X112" s="6"/>
+      <c r="X112" s="8"/>
     </row>
     <row r="113" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A113" s="5">
@@ -9030,7 +9495,9 @@
       <c r="U113" s="6"/>
       <c r="V113" s="6"/>
       <c r="W113" s="8"/>
-      <c r="X113" s="6"/>
+      <c r="X113" s="8" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="114" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A114" s="5">
@@ -9076,7 +9543,7 @@
       <c r="U114" s="6"/>
       <c r="V114" s="6"/>
       <c r="W114" s="8"/>
-      <c r="X114" s="6"/>
+      <c r="X114" s="8"/>
     </row>
     <row r="115" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
@@ -9122,7 +9589,9 @@
       <c r="U115" s="6"/>
       <c r="V115" s="6"/>
       <c r="W115" s="8"/>
-      <c r="X115" s="6"/>
+      <c r="X115" s="8" t="s">
+        <v>883</v>
+      </c>
     </row>
     <row r="116" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A116" s="5">
@@ -9168,7 +9637,9 @@
       <c r="U116" s="6"/>
       <c r="V116" s="6"/>
       <c r="W116" s="8"/>
-      <c r="X116" s="6"/>
+      <c r="X116" s="8" t="s">
+        <v>884</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9192,9 +9663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178334C-5EFE-4F48-9EA8-7AA58E735530}">
   <dimension ref="A1:B264"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -13257,8 +13726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF93574E-3500-41B6-8E4D-7ABAD002D051}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -13690,4 +14159,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B47F2D2-8379-4407-B6AE-B9221BBD032B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.07421875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="31">
+        <v>45619</v>
+      </c>
+      <c r="B2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="31">
+        <v>45643</v>
+      </c>
+      <c r="B3" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="31">
+        <v>45658</v>
+      </c>
+      <c r="B4" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="31">
+        <v>45664</v>
+      </c>
+      <c r="B5" t="s">
+        <v>813</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>